<commit_message>
updating config file with new paths
</commit_message>
<xml_diff>
--- a/data-generation/ConfigFiles/ConfigTest_Francois.xlsx
+++ b/data-generation/ConfigFiles/ConfigTest_Francois.xlsx
@@ -201,7 +201,7 @@
     <t xml:space="preserve">Demand</t>
   </si>
   <si>
-    <t xml:space="preserve">Database-matijs/TotalLoadValue_def/##/2019.csv</t>
+    <t xml:space="preserve">Database/TotalLoadValue_def/##/2019.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Flexible Demand</t>
@@ -216,7 +216,7 @@
     <t xml:space="preserve">Power plant data</t>
   </si>
   <si>
-    <t xml:space="preserve">Database-matijs/PowerPlants/##/JRC_EU_TIMES_ProRes1_2019_NOP2H_STO.csv</t>
+    <t xml:space="preserve">Database/PowerPlants/##/JRC_EU_TIMES_ProRes1_2019_NOP2H_STO.csv</t>
   </si>
   <si>
     <t xml:space="preserve">The path is an absolute path or a relative path to this config file</t>
@@ -225,7 +225,7 @@
     <t xml:space="preserve">Renewables AF</t>
   </si>
   <si>
-    <t xml:space="preserve">Database-matijs/AvailabilityFactors/##/2019.csv</t>
+    <t xml:space="preserve">Database/AvailabilityFactors/##/2019.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Load Shedding</t>
@@ -237,7 +237,7 @@
     <t xml:space="preserve">NTC</t>
   </si>
   <si>
-    <t xml:space="preserve">Database-matijs/DayAheadNTC/NTC_Matijs.csv</t>
+    <t xml:space="preserve">Database/DayAheadNTC/NTC_Matijs.csv</t>
   </si>
   <si>
     <t xml:space="preserve">for example: </t>
@@ -252,7 +252,7 @@
     <t xml:space="preserve">Scaled inflows</t>
   </si>
   <si>
-    <t xml:space="preserve">Database-matijs/ScaledInflows/##/lisflood_scaled_inflow_2015.csv</t>
+    <t xml:space="preserve">Database/ScaledInflows/##/lisflood_scaled_inflow_2015.csv</t>
   </si>
   <si>
     <t xml:space="preserve">will fetch one load.csv file per country, by replacing ## with FR, DE, NL, etc.</t>
@@ -264,19 +264,19 @@
     <t xml:space="preserve">Heat Demand</t>
   </si>
   <si>
-    <t xml:space="preserve">Database-matijs/HeatDemandTotal/HeatDemand_TOTAL.csv</t>
+    <t xml:space="preserve">Database/HeatDemandTotal/HeatDemand_TOTAL.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Temperatures</t>
   </si>
   <si>
-    <t xml:space="preserve">Database-matijs/Temperatures/Temps_2019.csv</t>
+    <t xml:space="preserve">Database/Temperatures/Temps_2019.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Geo Data</t>
   </si>
   <si>
-    <t xml:space="preserve">Database-matijs/ZonalData/geo_data_v2.csv</t>
+    <t xml:space="preserve">Database/ZonalData/geo_data_v2.csv</t>
   </si>
   <si>
     <t xml:space="preserve">H2 Demand (P2H2 - rigid)</t>
@@ -1087,7 +1087,43 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9D7A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1201,8 +1237,8 @@
   </sheetPr>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B175" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H235" activeCellId="0" sqref="H235"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F37" activeCellId="5" sqref="C125 C128:C129 C131 C133 C135:C137 F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3523,190 +3559,190 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <conditionalFormatting sqref="C79 C306:C320 C35:C36 C226:D247 F226:G247">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="5">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="1">
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="6">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="2">
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="7">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="3">
+    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="41">
-    <dataValidation allowBlank="true" operator="between" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files.&#10;&#10;The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" promptTitle="Path the simulation directory" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C34:D34" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files.&#10;&#10;The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" promptTitle="Path the simulation directory" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C34:D34" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." promptTitle="Start day of the simulation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C57" type="date">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." promptTitle="Start day of the simulation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C57" type="date">
       <formula1>1</formula1>
       <formula2>73051</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This is the last simulated day. It must be comprised within the range of dates provided within the data files." promptTitle="Stop day of the simulation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C58" type="date">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This is the last simulated day. It must be comprised within the range of dates provided within the data files." promptTitle="Stop day of the simulation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C58" type="date">
       <formula1>1</formula1>
       <formula2>73051</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Historical flows" promptTitle="Historical interconnection flows" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C132" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Historical flows" promptTitle="Historical interconnection flows" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C132" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="In case no data file is provided. This single value is used for all the sets." promptTitle="Default value" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F181:F187" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="In case no data file is provided. This single value is used for all the sets." promptTitle="Default value" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F181:F187" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" promptTitle="Multiplicative Factor" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C275" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" promptTitle="Multiplicative Factor" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C275" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" promptTitle="Multiplicative Factor" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C276" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" promptTitle="Multiplicative Factor" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C276" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" promptTitle="Multiplicative Factor" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C277" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" promptTitle="Multiplicative Factor" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C277" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" promptTitle="Multiplicative Factor" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C278" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" promptTitle="Multiplicative Factor" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C278" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Example:&#10;C:\GAMS\win64\24.3&#10;&#10;If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " promptTitle="Path to the gams folder" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C37" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Example:&#10;C:\GAMS\win64\24.3&#10;&#10;If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " promptTitle="Path to the gams folder" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C37" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="In case no data file is provided. This single value is used for all the sets.&#10;It is defined in % of the maximum load throughout the simulation period." promptTitle="Default value (% of max load)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F130" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="In case no data file is provided. This single value is used for all the sets.&#10;It is defined in % of the maximum load throughout the simulation period." promptTitle="Default value (% of max load)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F130" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="In case no data file is provided. This single value is used for all the sets." promptTitle="Default value (in EUR/t_co2)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F167:F168 F171:F172" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="In case no data file is provided. This single value is used for all the sets." promptTitle="Default value (in EUR/t_co2)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F167:F168 F171:F172" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases.&#10;&#10;Example:&#10;C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" promptTitle="Path to the cplex executable" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C38" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases.&#10;&#10;Example:&#10;C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" promptTitle="Path to the cplex executable" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C38" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" promptTitle="Reservoir inflows in MWh" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C133 C135:C136" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" promptTitle="Reservoir inflows in MWh" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C133 C135:C136" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Select the path the outage csv file from the database.&#10;&#10;The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" promptTitle="Path the outage data" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C127" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Select the path the outage csv file from the database.&#10;&#10;The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" promptTitle="Path the outage data" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C127" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This is the overlap period between consecutive optimization of the rolling horizon.&#10;&#10;If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" promptTitle="Look Ahead Period" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C60 C62" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This is the overlap period between consecutive optimization of the rolling horizon.&#10;&#10;If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" promptTitle="Look Ahead Period" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C60 C62" type="decimal">
       <formula1>0</formula1>
       <formula2>365</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This is the number of days to be optimized in the rolling horizon framework. Does not include the overlap period with the next optimization horizon. &#10;&#10;If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" promptTitle="Horizon length" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C59 C61" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This is the number of days to be optimized in the rolling horizon framework. Does not include the overlap period with the next optimization horizon. &#10;&#10;If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" promptTitle="Horizon length" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C59 C61" type="decimal">
       <formula1>1</formula1>
       <formula2>365</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" promptTitle="Load Shedding Costs" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F169" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" promptTitle="Load Shedding Costs" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F169" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " promptTitle="Value of Lost Load" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F205" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " promptTitle="Value of Lost Load" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F205" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" promptTitle="Price of spillage" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F206" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" promptTitle="Price of spillage" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F206" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" promptTitle="Water Value" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F207" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" promptTitle="Water Value" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F207" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Initial state of charge. It is defined as the % of total storage capacity." promptTitle="Default value (% of max storage)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F102" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Initial state of charge. It is defined as the % of total storage capacity." promptTitle="Default value (% of max storage)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F102" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="FInal state of charge. It is defined as the % of total storage capacity." promptTitle="Default value (% of max storage)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F103" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="FInal state of charge. It is defined as the % of total storage capacity." promptTitle="Default value (% of max storage)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F103" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" promptTitle="Flexible demand input file" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C126" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" promptTitle="Flexible demand input file" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C126" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" promptTitle="Flexible demand default value" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F126" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" promptTitle="Flexible demand default value" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F126" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="between 0 and 1" promptTitle="Share of 2U quick start units" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F164" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="between 0 and 1" promptTitle="Share of 2U quick start units" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F164" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Number of hours by which the flexible demand can be shifted" promptTitle="Demand flexiblity" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F163" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Number of hours by which the flexible demand can be shifted" promptTitle="Demand flexiblity" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F163" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" promptTitle="Defaut transmission price" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F170" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" promptTitle="Defaut transmission price" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F170" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" promptTitle="Transmission price" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C170" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" promptTitle="Transmission price" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C170" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Path to the time series for each zone.&#10;The unit should be MW&#10;If not provided, a standard formula is used to evaluate the reserve needs" promptTitle="Reserve down requirements" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C162" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Path to the time series for each zone.&#10;The unit should be MW&#10;If not provided, a standard formula is used to evaluate the reserve needs" promptTitle="Reserve down requirements" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C162" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Path to the time series for each zone.&#10;The unit should be MW&#10;If not provided, a standard formula is used to evaluate the reserve needs" promptTitle="Reserve up requirements" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C161" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Path to the time series for each zone.&#10;The unit should be MW&#10;If not provided, a standard formula is used to evaluate the reserve needs" promptTitle="Reserve up requirements" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C161" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Time series, expressed in MWh!" promptTitle="Demand for Hydrogen" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C137:C138" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Time series, expressed in MWh!" promptTitle="Demand for Hydrogen" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C137:C138" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C226:D247 F226:G247 C306:C320" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C226:D247 F226:G247 C306:C320" type="list">
       <formula1>Lists!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." promptTitle="Write GDX file" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C35:D35" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." promptTitle="Write GDX file" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C35:D35" type="list">
       <formula1>Lists!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="If set to true, one pickle file (python data format) is written in the simulation environment directory to allow quickly retrieving the simulation inputs" promptTitle="Write Pickles file" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C36:D36 D76" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="If set to true, one pickle file (python data format) is written in the simulation environment directory to allow quickly retrieving the simulation inputs" promptTitle="Write Pickles file" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C36:D36 D76" type="list">
       <formula1>Lists!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This inputs allows selecting the metodology for reserve sizing&#10;" promptTitle="Reserve Calculation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C78" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="This inputs allows selecting the metodology for reserve sizing&#10;" promptTitle="Reserve Calculation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C78" type="list">
       <formula1>Lists!$C$2:$C$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Set to true to allow curtailment" promptTitle="Allow Curtailment of Renewables" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C79" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Set to true to allow curtailment" promptTitle="Allow Curtailment of Renewables" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C79" type="list">
       <formula1>Lists!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Select the type of optimization to perform." promptTitle="Simulation type" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C77" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Select the type of optimization to perform." promptTitle="Simulation type" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C77" type="list">
       <formula1>Lists!$B$2:$B$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Select type of mid-term hydro scheduling.&#10;Off: Mid-term scheduling is not performed, hystorical reservoir levels are used instead&#10;Regional: Performed for the whole region simultaneously&#10;Zonal: Performed for each zone individually" promptTitle="Hydro Scheduling" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C99" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Select type of mid-term hydro scheduling.&#10;Off: Mid-term scheduling is not performed, hystorical reservoir levels are used instead&#10;Regional: Performed for the whole region simultaneously&#10;Zonal: Performed for each zone individually" promptTitle="Hydro Scheduling" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C99" type="list">
       <formula1>Lists!$E$2:$E$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Annual: Performes hydro scheduling for one year&#10;Stop-date driven: Performes hydro scheduling between Start and Stop dates&#10;" promptTitle="Hydro scheduling horizon" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Annual: Performes hydro scheduling for one year&#10;Stop-date driven: Performes hydro scheduling between Start and Stop dates&#10;" promptTitle="Hydro scheduling horizon" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C100" type="list">
       <formula1>Lists!$F$2:$F$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Values for the initial and final levels, usefull when no reservoir levels are proided as inputs in the Input data" promptTitle="Initial/Final reservoir levels" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C101" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Values for the initial and final levels, usefull when no reservoir levels are proided as inputs in the Input data" promptTitle="Initial/Final reservoir levels" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C101" type="list">
       <formula1>Lists!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3722,7 +3758,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="5" sqref="C125 C128:C129 C131 C133 C135:C137 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3819,8 +3855,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3836,7 +3872,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="5" sqref="C125 C128:C129 C131 C133 C135:C137 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4805,22 +4841,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="4">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="9">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="5">
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="10">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:O16" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:O16" type="list">
       <formula1>Lists!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>